<commit_message>
ui changes are done
</commit_message>
<xml_diff>
--- a/backend-Planner/data/planner_agent_data_nushan.xlsx
+++ b/backend-Planner/data/planner_agent_data_nushan.xlsx
@@ -41794,10 +41794,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44888,18 +44888,6 @@
       <c r="I97" t="str">
         <f>LEFT(F97,2)</f>
         <v>IS</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
-      <c r="D98">
-        <f>SUM(D2:D97)</f>
-        <v>235</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9">
-      <c r="D99">
-        <f>SUM(D75:D97)</f>
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>